<commit_message>
Ethanol plant life, NCapTlife from 30 to 40
</commit_message>
<xml_diff>
--- a/Inputs/Ethanol.xlsx
+++ b/Inputs/Ethanol.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SugarModel\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\models\SugarModel\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64B739CD-F47A-4187-B7D3-3B791B21C61F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2925" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{7938D4A6-2C27-41D6-93C0-6D919A23BA1E}"/>
+    <workbookView xWindow="5250" yWindow="2925" windowWidth="21600" windowHeight="11385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Processes_ETHANOL1GEN" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,12 +38,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ken Noble</author>
   </authors>
   <commentList>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{9A25D4C5-E7F1-4DF3-B649-43B15F6D95F1}">
+    <comment ref="G7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,35 +62,56 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={8F64E3CE-28AB-447F-8A7D-CD8A72ED0013}</author>
     <author>tc={78B360FA-39D7-4F51-AB8F-EF995CC1C230}</author>
     <author>tc={91342960-EF99-4359-9548-EF08F5B3BB67}</author>
   </authors>
   <commentList>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{8F64E3CE-28AB-447F-8A7D-CD8A72ED0013}">
+    <comment ref="D17" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     2011 Rands</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C35" authorId="1" shapeId="0" xr:uid="{78B360FA-39D7-4F51-AB8F-EF995CC1C230}">
+    <comment ref="C35" authorId="1" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Includes treatment of CMS</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C46" authorId="2" shapeId="0" xr:uid="{91342960-EF99-4359-9548-EF08F5B3BB67}">
+    <comment ref="C46" authorId="2" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Assuming final stage Sugar Refining and ethanol production require same amount of steam (as per Tait 2014).</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -404,12 +424,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -488,12 +508,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -605,9 +619,9 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 13" xfId="6" xr:uid="{F01AFCFE-93C1-46AA-AD19-4BDED9351EDB}"/>
-    <cellStyle name="Normal 2" xfId="4" xr:uid="{E74171AD-E22A-4FD6-9898-06B1BDF6005E}"/>
-    <cellStyle name="Normal 2 2 2" xfId="5" xr:uid="{0E2DA0FF-5D17-46AE-8C84-BE106F480DE2}"/>
+    <cellStyle name="Normal 13" xfId="6"/>
+    <cellStyle name="Normal 2" xfId="4"/>
+    <cellStyle name="Normal 2 2 2" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -687,7 +701,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADAA76E5-5485-476D-B9C2-D47B1F3E791E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ADAA76E5-5485-476D-B9C2-D47B1F3E791E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -745,7 +759,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8F38FE7-9C87-4783-80A3-22581C894C2E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E8F38FE7-9C87-4783-80A3-22581C894C2E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -803,7 +817,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EB5CE23-A341-46C3-836F-AC6BB29D693A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6EB5CE23-A341-46C3-836F-AC6BB29D693A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -866,7 +880,7 @@
                   <a14:compatExt spid="_x0000_s2049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B482974-3333-403A-8DD6-BC66FA842BAA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0B482974-3333-403A-8DD6-BC66FA842BAA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -924,7 +938,7 @@
                   <a14:compatExt spid="_x0000_s2050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4629A7E0-FCFC-4522-A8C1-C40E68C65926}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4629A7E0-FCFC-4522-A8C1-C40E68C65926}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -982,7 +996,7 @@
                   <a14:compatExt spid="_x0000_s2051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11312D87-5018-4D95-A4E2-FF375FC5C2BD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{11312D87-5018-4D95-A4E2-FF375FC5C2BD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1040,7 +1054,7 @@
                   <a14:compatExt spid="_x0000_s2052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1734D898-47DD-4F1F-A926-0E0690ABA003}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1734D898-47DD-4F1F-A926-0E0690ABA003}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1098,7 +1112,7 @@
                   <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0B1CEF1-FBDF-4A37-A7E0-1323B2691974}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0B1CEF1-FBDF-4A37-A7E0-1323B2691974}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1156,7 +1170,7 @@
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E553EB3C-8F09-4DE4-9471-BD58C1EBC09E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E553EB3C-8F09-4DE4-9471-BD58C1EBC09E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1214,7 +1228,7 @@
                   <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96EF8E9B-6046-454B-ADC3-91FE0A58D1FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96EF8E9B-6046-454B-ADC3-91FE0A58D1FE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1272,7 +1286,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97C2C67F-F6AC-41B1-8F5D-3851FB085C5A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{97C2C67F-F6AC-41B1-8F5D-3851FB085C5A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1316,7 +1330,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BE9C859-0BB9-48BC-9557-4FA528F7A230}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9BE9C859-0BB9-48BC-9557-4FA528F7A230}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1374,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09BE8708-843B-4A9D-BF38-11A9C53398A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{09BE8708-843B-4A9D-BF38-11A9C53398A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1404,7 +1418,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48C127DA-4566-4090-8C34-12BDB6889DFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{48C127DA-4566-4090-8C34-12BDB6889DFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1448,7 +1462,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24C90138-5127-40F4-B501-92BAE8CB79EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{24C90138-5127-40F4-B501-92BAE8CB79EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1492,7 +1506,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2ECE3D9-8C21-4CB8-A61E-837286C3072C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2ECE3D9-8C21-4CB8-A61E-837286C3072C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2029,7 +2043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291E7F2D-A250-455E-94C6-6C530676ADB3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -2377,18 +2391,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="1025" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2397,7 +2411,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="1025" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2427,18 +2441,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="1027" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2447,7 +2461,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="1027" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2455,7 +2469,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682A5139-1D21-407D-947D-FB21F5957273}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet32">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -2465,7 +2479,7 @@
       <pane xSplit="7" ySplit="7" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2692,7 +2706,7 @@
         <v>0.8</v>
       </c>
       <c r="M9" s="13">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="N9" s="13">
         <v>2025</v>
@@ -2833,43 +2847,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2055" r:id="rId4" name="cmdAddParamQualifier2">
+        <control shapeId="2049" r:id="rId4" name="cmdTechNameAndDesc">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2055" r:id="rId4" name="cmdAddParamQualifier2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2054" r:id="rId6" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>847725</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -2878,32 +2867,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2054" r:id="rId6" name="cmdCheckTechDataSheet"/>
+        <control shapeId="2049" r:id="rId4" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2053" r:id="rId8" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="2050" r:id="rId6" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2053" r:id="rId8" name="cmdAddParamQualifier1"/>
+        <control shapeId="2050" r:id="rId6" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2051" r:id="rId8" name="cmdCommOUT">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2051" r:id="rId8" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2933,18 +2947,43 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2051" r:id="rId12" name="cmdCommOUT">
+        <control shapeId="2053" r:id="rId12" name="cmdAddParamQualifier1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2053" r:id="rId12" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2054" r:id="rId14" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -2953,57 +2992,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2051" r:id="rId12" name="cmdCommOUT"/>
+        <control shapeId="2054" r:id="rId14" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2050" r:id="rId14" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+        <control shapeId="2055" r:id="rId16" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2050" r:id="rId14" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId16" name="cmdTechNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>847725</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2049" r:id="rId16" name="cmdTechNameAndDesc"/>
+        <control shapeId="2055" r:id="rId16" name="cmdAddParamQualifier2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3011,7 +3025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DA6C35-E768-455A-A0E4-E8C44D22DB15}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>

</xml_diff>

<commit_message>
ethanol plant life scenarios: 10;40
</commit_message>
<xml_diff>
--- a/Inputs/Ethanol.xlsx
+++ b/Inputs/Ethanol.xlsx
@@ -1579,19 +1579,10 @@
       <sheetName val="ANSv2-692-TS&amp;TID TRADE"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="6">
-          <cell r="E6">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="2">
-          <cell r="E2" t="str">
-            <v>INDCOA</v>
-          </cell>
           <cell r="R2" t="str">
             <v>BCS</v>
           </cell>
@@ -1622,15 +1613,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
       <sheetData sheetId="6">
-        <row r="5">
-          <cell r="F5">
-            <v>5.3887278299999997</v>
-          </cell>
-        </row>
         <row r="16">
           <cell r="K16">
             <v>47.206842041346803</v>
@@ -1647,23 +1633,17 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9">
-        <row r="23">
-          <cell r="C23">
-            <v>0.236875</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
       <sheetData sheetId="18">
         <row r="1">
           <cell r="B1" t="str">
@@ -1671,10 +1651,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
       <sheetData sheetId="23">
         <row r="27">
           <cell r="A27" t="str">
@@ -1682,15 +1662,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
       <sheetData sheetId="27">
-        <row r="17">
-          <cell r="P17">
-            <v>55.383497973610311</v>
-          </cell>
-        </row>
         <row r="32">
           <cell r="AF32">
             <v>0.17597823500185439</v>
@@ -1712,16 +1687,16 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>